<commit_message>
feat: 自动添加每日生成文件 AIPEFinanceData.xlsx (Colab)
</commit_message>
<xml_diff>
--- a/AIPEPortfolio.xlsx
+++ b/AIPEPortfolio.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1305,16 +1305,407 @@
         <v>202507011425</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B54" t="str">
+        <v>600900</v>
+      </c>
+      <c r="C54" t="str">
+        <v>长江电力</v>
+      </c>
+      <c r="D54">
+        <v>17</v>
+      </c>
+      <c r="E54" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B55" t="str">
+        <v>000333</v>
+      </c>
+      <c r="C55" t="str">
+        <v>美的集团</v>
+      </c>
+      <c r="D55">
+        <v>3.06</v>
+      </c>
+      <c r="E55" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B56" t="str">
+        <v>518880</v>
+      </c>
+      <c r="C56" t="str">
+        <v>黄金ETF</v>
+      </c>
+      <c r="D56">
+        <v>4.88</v>
+      </c>
+      <c r="E56" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B57" t="str">
+        <v>510300</v>
+      </c>
+      <c r="C57" t="str">
+        <v>沪深300ETF</v>
+      </c>
+      <c r="D57">
+        <v>5.01</v>
+      </c>
+      <c r="E57" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B58" t="str">
+        <v>HK02899</v>
+      </c>
+      <c r="C58" t="str">
+        <v>紫金矿业</v>
+      </c>
+      <c r="D58">
+        <v>9.89</v>
+      </c>
+      <c r="E58" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B59" t="str">
+        <v>HK06881</v>
+      </c>
+      <c r="C59" t="str">
+        <v>中国银河</v>
+      </c>
+      <c r="D59">
+        <v>5.22</v>
+      </c>
+      <c r="E59" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B60" t="str">
+        <v>510050</v>
+      </c>
+      <c r="C60" t="str">
+        <v>上证50ETF</v>
+      </c>
+      <c r="D60">
+        <v>5.14</v>
+      </c>
+      <c r="E60" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B61" t="str">
+        <v>600085</v>
+      </c>
+      <c r="C61" t="str">
+        <v>同仁堂</v>
+      </c>
+      <c r="D61">
+        <v>1.98</v>
+      </c>
+      <c r="E61" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B62" t="str">
+        <v>600989</v>
+      </c>
+      <c r="C62" t="str">
+        <v>宝丰能源</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B63" t="str">
+        <v>601899</v>
+      </c>
+      <c r="C63" t="str">
+        <v>紫金矿业</v>
+      </c>
+      <c r="D63">
+        <v>9.92</v>
+      </c>
+      <c r="E63" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B64" t="str">
+        <v>601688</v>
+      </c>
+      <c r="C64" t="str">
+        <v>华泰证券</v>
+      </c>
+      <c r="D64">
+        <v>5</v>
+      </c>
+      <c r="E64" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B65" t="str">
+        <v>600900</v>
+      </c>
+      <c r="C65" t="str">
+        <v>长江电力</v>
+      </c>
+      <c r="D65">
+        <v>17</v>
+      </c>
+      <c r="E65" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B66" t="str">
+        <v>000333</v>
+      </c>
+      <c r="C66" t="str">
+        <v>美的集团</v>
+      </c>
+      <c r="D66">
+        <v>3.06</v>
+      </c>
+      <c r="E66" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B67" t="str">
+        <v>518880</v>
+      </c>
+      <c r="C67" t="str">
+        <v>黄金ETF</v>
+      </c>
+      <c r="D67">
+        <v>4.88</v>
+      </c>
+      <c r="E67" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B68" t="str">
+        <v>510300</v>
+      </c>
+      <c r="C68" t="str">
+        <v>沪深300ETF</v>
+      </c>
+      <c r="D68">
+        <v>5.01</v>
+      </c>
+      <c r="E68" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B69" t="str">
+        <v>HK02899</v>
+      </c>
+      <c r="C69" t="str">
+        <v>紫金矿业</v>
+      </c>
+      <c r="D69">
+        <v>9.89</v>
+      </c>
+      <c r="E69" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B70" t="str">
+        <v>HK06881</v>
+      </c>
+      <c r="C70" t="str">
+        <v>中国银河</v>
+      </c>
+      <c r="D70">
+        <v>5.22</v>
+      </c>
+      <c r="E70" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B71" t="str">
+        <v>510050</v>
+      </c>
+      <c r="C71" t="str">
+        <v>上证50ETF</v>
+      </c>
+      <c r="D71">
+        <v>5.14</v>
+      </c>
+      <c r="E71" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B72" t="str">
+        <v>600085</v>
+      </c>
+      <c r="C72" t="str">
+        <v>同仁堂</v>
+      </c>
+      <c r="D72">
+        <v>1.98</v>
+      </c>
+      <c r="E72" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B73" t="str">
+        <v>600989</v>
+      </c>
+      <c r="C73" t="str">
+        <v>宝丰能源</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B74" t="str">
+        <v>601899</v>
+      </c>
+      <c r="C74" t="str">
+        <v>紫金矿业</v>
+      </c>
+      <c r="D74">
+        <v>9.92</v>
+      </c>
+      <c r="E74" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B75" t="str">
+        <v>601688</v>
+      </c>
+      <c r="C75" t="str">
+        <v>华泰证券</v>
+      </c>
+      <c r="D75">
+        <v>5</v>
+      </c>
+      <c r="E75" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>大智 (稳健智远)</v>
+      </c>
+      <c r="B76" t="str">
+        <v>600380</v>
+      </c>
+      <c r="C76" t="str">
+        <v>健康元</v>
+      </c>
+      <c r="D76">
+        <v>10</v>
+      </c>
+      <c r="E76" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E53"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E76"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1897,16 +2288,254 @@
         <v>202507011425</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B35" t="str">
+        <v>603119</v>
+      </c>
+      <c r="C35" t="str">
+        <v>浙江荣泰</v>
+      </c>
+      <c r="D35">
+        <v>42.95</v>
+      </c>
+      <c r="E35" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B36" t="str">
+        <v>688290</v>
+      </c>
+      <c r="C36" t="str">
+        <v>景业智能</v>
+      </c>
+      <c r="D36">
+        <v>7.46</v>
+      </c>
+      <c r="E36" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B37" t="str">
+        <v>513100</v>
+      </c>
+      <c r="C37" t="str">
+        <v>纳指ETF</v>
+      </c>
+      <c r="D37">
+        <v>4.85</v>
+      </c>
+      <c r="E37" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B38" t="str">
+        <v>513290</v>
+      </c>
+      <c r="C38" t="str">
+        <v>纳指生物科技ETF</v>
+      </c>
+      <c r="D38">
+        <v>0.93</v>
+      </c>
+      <c r="E38" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B39" t="str">
+        <v>000725</v>
+      </c>
+      <c r="C39" t="str">
+        <v>京东方A</v>
+      </c>
+      <c r="D39">
+        <v>4.84</v>
+      </c>
+      <c r="E39" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B40" t="str">
+        <v>159781</v>
+      </c>
+      <c r="C40" t="str">
+        <v>科创创业ETF</v>
+      </c>
+      <c r="D40">
+        <v>9.93</v>
+      </c>
+      <c r="E40" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B41" t="str">
+        <v>HK01896</v>
+      </c>
+      <c r="C41" t="str">
+        <v>猫眼娱乐</v>
+      </c>
+      <c r="D41">
+        <v>0.97</v>
+      </c>
+      <c r="E41" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B42" t="str">
+        <v>603119</v>
+      </c>
+      <c r="C42" t="str">
+        <v>浙江荣泰</v>
+      </c>
+      <c r="D42">
+        <v>42.95</v>
+      </c>
+      <c r="E42" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B43" t="str">
+        <v>688290</v>
+      </c>
+      <c r="C43" t="str">
+        <v>景业智能</v>
+      </c>
+      <c r="D43">
+        <v>7.46</v>
+      </c>
+      <c r="E43" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B44" t="str">
+        <v>513100</v>
+      </c>
+      <c r="C44" t="str">
+        <v>纳指ETF</v>
+      </c>
+      <c r="D44">
+        <v>4.85</v>
+      </c>
+      <c r="E44" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B45" t="str">
+        <v>513290</v>
+      </c>
+      <c r="C45" t="str">
+        <v>纳指生物科技ETF</v>
+      </c>
+      <c r="D45">
+        <v>0.93</v>
+      </c>
+      <c r="E45" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B46" t="str">
+        <v>000725</v>
+      </c>
+      <c r="C46" t="str">
+        <v>京东方A</v>
+      </c>
+      <c r="D46">
+        <v>4.84</v>
+      </c>
+      <c r="E46" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B47" t="str">
+        <v>159781</v>
+      </c>
+      <c r="C47" t="str">
+        <v>科创创业ETF</v>
+      </c>
+      <c r="D47">
+        <v>9.93</v>
+      </c>
+      <c r="E47" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>大成 (锐进先锋)</v>
+      </c>
+      <c r="B48" t="str">
+        <v>HK01896</v>
+      </c>
+      <c r="C48" t="str">
+        <v>猫眼娱乐</v>
+      </c>
+      <c r="D48">
+        <v>0.97</v>
+      </c>
+      <c r="E48" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E34"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E48"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -3751,9 +4380,814 @@
         <v>202507011425</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B81" t="str">
+        <v>600900</v>
+      </c>
+      <c r="C81" t="str">
+        <v>长江电力</v>
+      </c>
+      <c r="D81" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E81">
+        <v>30.04</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B82" t="str">
+        <v>000333</v>
+      </c>
+      <c r="C82" t="str">
+        <v>美的集团</v>
+      </c>
+      <c r="D82" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E82">
+        <v>3.06</v>
+      </c>
+      <c r="F82">
+        <v>1.02</v>
+      </c>
+      <c r="G82" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B83" t="str">
+        <v>603119</v>
+      </c>
+      <c r="C83" t="str">
+        <v>浙江荣泰</v>
+      </c>
+      <c r="D83" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E83">
+        <v>42.8</v>
+      </c>
+      <c r="F83">
+        <v>1.14</v>
+      </c>
+      <c r="G83" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B84" t="str">
+        <v>518880</v>
+      </c>
+      <c r="C84" t="str">
+        <v>黄金ETF</v>
+      </c>
+      <c r="D84" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E84">
+        <v>4.87</v>
+      </c>
+      <c r="F84">
+        <v>0.98</v>
+      </c>
+      <c r="G84" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B85" t="str">
+        <v>510300</v>
+      </c>
+      <c r="C85" t="str">
+        <v>沪深300ETF</v>
+      </c>
+      <c r="D85" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E85">
+        <v>5.01</v>
+      </c>
+      <c r="F85">
+        <v>5</v>
+      </c>
+      <c r="G85" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B86" t="str">
+        <v>513100</v>
+      </c>
+      <c r="C86" t="str">
+        <v>纳指ETF</v>
+      </c>
+      <c r="D86" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E86">
+        <v>4.87</v>
+      </c>
+      <c r="F86">
+        <v>1.02</v>
+      </c>
+      <c r="G86" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B87" t="str">
+        <v>HK06881</v>
+      </c>
+      <c r="C87" t="str">
+        <v>中国银河</v>
+      </c>
+      <c r="D87" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E87">
+        <v>5.22</v>
+      </c>
+      <c r="F87">
+        <v>1.05</v>
+      </c>
+      <c r="G87" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B88" t="str">
+        <v>510050</v>
+      </c>
+      <c r="C88" t="str">
+        <v>上证50ETF</v>
+      </c>
+      <c r="D88" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E88">
+        <v>5.14</v>
+      </c>
+      <c r="F88">
+        <v>5.14</v>
+      </c>
+      <c r="G88" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B89" t="str">
+        <v>600085</v>
+      </c>
+      <c r="C89" t="str">
+        <v>同仁堂</v>
+      </c>
+      <c r="D89" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E89">
+        <v>1.98</v>
+      </c>
+      <c r="F89">
+        <v>0.99</v>
+      </c>
+      <c r="G89" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B90" t="str">
+        <v>513290</v>
+      </c>
+      <c r="C90" t="str">
+        <v>纳指生物科技ETF</v>
+      </c>
+      <c r="D90" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E90">
+        <v>0.93</v>
+      </c>
+      <c r="F90">
+        <v>0.98</v>
+      </c>
+      <c r="G90" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B91" t="str">
+        <v>000725</v>
+      </c>
+      <c r="C91" t="str">
+        <v>京东方A</v>
+      </c>
+      <c r="D91" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E91">
+        <v>4.84</v>
+      </c>
+      <c r="F91">
+        <v>5.09</v>
+      </c>
+      <c r="G91" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B92" t="str">
+        <v>159781</v>
+      </c>
+      <c r="C92" t="str">
+        <v>科创创业ETF</v>
+      </c>
+      <c r="D92" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E92">
+        <v>9.96</v>
+      </c>
+      <c r="F92">
+        <v>5.25</v>
+      </c>
+      <c r="G92" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B93" t="str">
+        <v>600989</v>
+      </c>
+      <c r="C93" t="str">
+        <v>宝丰能源</v>
+      </c>
+      <c r="D93" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E93">
+        <v>4.8</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B94" t="str">
+        <v>601899</v>
+      </c>
+      <c r="C94" t="str">
+        <v>紫金矿业</v>
+      </c>
+      <c r="D94" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E94">
+        <v>9.91</v>
+      </c>
+      <c r="F94">
+        <v>9.91</v>
+      </c>
+      <c r="G94" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B95" t="str">
+        <v>HK02899</v>
+      </c>
+      <c r="C95" t="str">
+        <v>紫金矿业</v>
+      </c>
+      <c r="D95" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E95">
+        <v>9.89</v>
+      </c>
+      <c r="F95">
+        <v>1.11</v>
+      </c>
+      <c r="G95" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B96" t="str">
+        <v>688290</v>
+      </c>
+      <c r="C96" t="str">
+        <v>景业智能</v>
+      </c>
+      <c r="D96" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E96">
+        <v>7.46</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B97" t="str">
+        <v>HK01896</v>
+      </c>
+      <c r="C97" t="str">
+        <v>猫眼娱乐</v>
+      </c>
+      <c r="D97" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E97">
+        <v>0.97</v>
+      </c>
+      <c r="F97">
+        <v>0.2</v>
+      </c>
+      <c r="G97" t="str">
+        <v>202507021030</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B98" t="str">
+        <v>600900</v>
+      </c>
+      <c r="C98" t="str">
+        <v>长江电力</v>
+      </c>
+      <c r="D98" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E98">
+        <v>17</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B99" t="str">
+        <v>000333</v>
+      </c>
+      <c r="C99" t="str">
+        <v>美的集团</v>
+      </c>
+      <c r="D99" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E99">
+        <v>3.06</v>
+      </c>
+      <c r="F99">
+        <v>1.02</v>
+      </c>
+      <c r="G99" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B100" t="str">
+        <v>603119</v>
+      </c>
+      <c r="C100" t="str">
+        <v>浙江荣泰</v>
+      </c>
+      <c r="D100" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E100">
+        <v>42.95</v>
+      </c>
+      <c r="F100">
+        <v>1.14</v>
+      </c>
+      <c r="G100" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B101" t="str">
+        <v>518880</v>
+      </c>
+      <c r="C101" t="str">
+        <v>黄金ETF</v>
+      </c>
+      <c r="D101" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E101">
+        <v>4.88</v>
+      </c>
+      <c r="F101">
+        <v>0.98</v>
+      </c>
+      <c r="G101" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B102" t="str">
+        <v>510300</v>
+      </c>
+      <c r="C102" t="str">
+        <v>沪深300ETF</v>
+      </c>
+      <c r="D102" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E102">
+        <v>5.01</v>
+      </c>
+      <c r="F102">
+        <v>5</v>
+      </c>
+      <c r="G102" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B103" t="str">
+        <v>513100</v>
+      </c>
+      <c r="C103" t="str">
+        <v>纳指ETF</v>
+      </c>
+      <c r="D103" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E103">
+        <v>4.85</v>
+      </c>
+      <c r="F103">
+        <v>1.02</v>
+      </c>
+      <c r="G103" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B104" t="str">
+        <v>HK06881</v>
+      </c>
+      <c r="C104" t="str">
+        <v>中国银河</v>
+      </c>
+      <c r="D104" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E104">
+        <v>5.22</v>
+      </c>
+      <c r="F104">
+        <v>1.05</v>
+      </c>
+      <c r="G104" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B105" t="str">
+        <v>510050</v>
+      </c>
+      <c r="C105" t="str">
+        <v>上证50ETF</v>
+      </c>
+      <c r="D105" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E105">
+        <v>5.14</v>
+      </c>
+      <c r="F105">
+        <v>5.14</v>
+      </c>
+      <c r="G105" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B106" t="str">
+        <v>600085</v>
+      </c>
+      <c r="C106" t="str">
+        <v>同仁堂</v>
+      </c>
+      <c r="D106" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E106">
+        <v>1.98</v>
+      </c>
+      <c r="F106">
+        <v>0.99</v>
+      </c>
+      <c r="G106" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B107" t="str">
+        <v>513290</v>
+      </c>
+      <c r="C107" t="str">
+        <v>纳指生物科技ETF</v>
+      </c>
+      <c r="D107" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E107">
+        <v>0.93</v>
+      </c>
+      <c r="F107">
+        <v>0.98</v>
+      </c>
+      <c r="G107" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B108" t="str">
+        <v>000725</v>
+      </c>
+      <c r="C108" t="str">
+        <v>京东方A</v>
+      </c>
+      <c r="D108" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E108">
+        <v>4.84</v>
+      </c>
+      <c r="F108">
+        <v>5.09</v>
+      </c>
+      <c r="G108" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B109" t="str">
+        <v>159781</v>
+      </c>
+      <c r="C109" t="str">
+        <v>科创创业ETF</v>
+      </c>
+      <c r="D109" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E109">
+        <v>9.93</v>
+      </c>
+      <c r="F109">
+        <v>5.25</v>
+      </c>
+      <c r="G109" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B110" t="str">
+        <v>600989</v>
+      </c>
+      <c r="C110" t="str">
+        <v>宝丰能源</v>
+      </c>
+      <c r="D110" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+      <c r="G110" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B111" t="str">
+        <v>601899</v>
+      </c>
+      <c r="C111" t="str">
+        <v>紫金矿业</v>
+      </c>
+      <c r="D111" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E111">
+        <v>9.92</v>
+      </c>
+      <c r="F111">
+        <v>9.91</v>
+      </c>
+      <c r="G111" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B112" t="str">
+        <v>HK02899</v>
+      </c>
+      <c r="C112" t="str">
+        <v>紫金矿业</v>
+      </c>
+      <c r="D112" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E112">
+        <v>9.89</v>
+      </c>
+      <c r="F112">
+        <v>1.11</v>
+      </c>
+      <c r="G112" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B113" t="str">
+        <v>HK01896</v>
+      </c>
+      <c r="C113" t="str">
+        <v>猫眼娱乐</v>
+      </c>
+      <c r="D113" t="str">
+        <v>大成</v>
+      </c>
+      <c r="E113">
+        <v>0.97</v>
+      </c>
+      <c r="F113">
+        <v>0.2</v>
+      </c>
+      <c r="G113" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B114" t="str">
+        <v>601688</v>
+      </c>
+      <c r="C114" t="str">
+        <v>华泰证券</v>
+      </c>
+      <c r="D114" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E114">
+        <v>5</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>范式进化投资组合</v>
+      </c>
+      <c r="B115" t="str">
+        <v>600380</v>
+      </c>
+      <c r="C115" t="str">
+        <v>健康元</v>
+      </c>
+      <c r="D115" t="str">
+        <v>大智</v>
+      </c>
+      <c r="E115">
+        <v>10</v>
+      </c>
+      <c r="F115">
+        <v>5</v>
+      </c>
+      <c r="G115" t="str">
+        <v>202507021326</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G80"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G115"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>